<commit_message>
Now can read HX-Express and SpecExport formats. Not yet implemented reading full TestSet
</commit_message>
<xml_diff>
--- a/Bimodal_HDX_Data/Timing.xlsx
+++ b/Bimodal_HDX_Data/Timing.xlsx
@@ -8,21 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/698444b0bac14488/Documents/My Documents/KlevitHahn/hdx-ms/pyHXExpress/Bimodal_HDX_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6E815C4085D7DFC9F9AE8D908361C68DA6FB2C96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{716FC620-2739-40BB-92F0-AAE9EB41794B}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_6E815C4085D7DFC9F9AE8D908361C68DA6FB2C96" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97DFBB16-615F-48CF-8BD0-E069DF916A2F}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13373" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15360" yWindow="0" windowWidth="15360" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>time point</t>
   </si>
@@ -250,6 +263,15 @@
   </si>
   <si>
     <t>pep124</t>
+  </si>
+  <si>
+    <t>start_seq</t>
+  </si>
+  <si>
+    <t>end_seq</t>
+  </si>
+  <si>
+    <t>peptide_range</t>
   </si>
 </sst>
 </file>
@@ -303,6 +325,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -592,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS28"/>
+  <dimension ref="A1:AS32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1059,7 +1085,7 @@
         <v>365.42396000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1079,7 +1105,7 @@
         <v>556.27</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1090,7 +1116,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>12</v>
       </c>
@@ -1101,7 +1127,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>13</v>
       </c>
@@ -1111,8 +1137,23 @@
       <c r="C20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>14</v>
       </c>
@@ -1122,8 +1163,25 @@
       <c r="C21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <f>LEN(H21)</f>
+        <v>8</v>
+      </c>
+      <c r="K21" t="str">
+        <f>_xlfn.CONCAT(TEXT(I21,"0000"),"-",TEXT(J21,"0000"))</f>
+        <v>0001-0008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>15</v>
       </c>
@@ -1133,8 +1191,25 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G22" t="s">
+        <v>68</v>
+      </c>
+      <c r="H22" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22:J32" si="0">LEN(H22)</f>
+        <v>15</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" ref="K22:K32" si="1">_xlfn.CONCAT(TEXT(I22,"0000"),"-",TEXT(J22,"0000"))</f>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>16</v>
       </c>
@@ -1144,8 +1219,25 @@
       <c r="C23" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>17</v>
       </c>
@@ -1155,8 +1247,25 @@
       <c r="C24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0009</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>18</v>
       </c>
@@ -1166,8 +1275,25 @@
       <c r="C25" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1177,8 +1303,25 @@
       <c r="C26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>20</v>
       </c>
@@ -1188,8 +1331,25 @@
       <c r="C27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>60</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>21</v>
       </c>
@@ -1198,6 +1358,99 @@
       </c>
       <c r="C28" t="s">
         <v>3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H28" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0014</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G29" t="s">
+        <v>73</v>
+      </c>
+      <c r="H29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" t="s">
+        <v>64</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G31" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" t="s">
+        <v>65</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0015</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G32" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" t="s">
+        <v>67</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="1"/>
+        <v>0001-0005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>